<commit_message>
Various things to do with the data files
</commit_message>
<xml_diff>
--- a/data/Horsager_2011/DataSummary_Horsager2011.xlsx
+++ b/data/Horsager_2011/DataSummary_Horsager2011.xlsx
@@ -586,7 +586,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,9 +600,7 @@
     <col min="7" max="7" width="11.140625" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="16" width="9.140625" style="1"/>
-    <col min="17" max="21" width="9.140625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="25" width="9.140625" style="1" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Small fix data files, beginning experimental code
</commit_message>
<xml_diff>
--- a/data/Horsager_2011/DataSummary_Horsager2011.xlsx
+++ b/data/Horsager_2011/DataSummary_Horsager2011.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="49">
   <si>
     <t>A1</t>
   </si>
@@ -87,48 +87,6 @@
   </si>
   <si>
     <t>S05_C1_D1</t>
-  </si>
-  <si>
-    <t>S05_C1_D4</t>
-  </si>
-  <si>
-    <t>S05_C1_D5</t>
-  </si>
-  <si>
-    <t>S05_C1_D6</t>
-  </si>
-  <si>
-    <t>S05_C1_D7</t>
-  </si>
-  <si>
-    <t>S05_C1_D8</t>
-  </si>
-  <si>
-    <t>S05_C1_D9</t>
-  </si>
-  <si>
-    <t>S05_C1_D10</t>
-  </si>
-  <si>
-    <t>S05_C1_D11</t>
-  </si>
-  <si>
-    <t>S05_C1_D12</t>
-  </si>
-  <si>
-    <t>S05_C1_D13</t>
-  </si>
-  <si>
-    <t>S05_C1_D14</t>
-  </si>
-  <si>
-    <t>S05_C1_D15</t>
-  </si>
-  <si>
-    <t>S05_C1_D16</t>
-  </si>
-  <si>
-    <t>S05_C1_D17</t>
   </si>
   <si>
     <t>delay (ms)</t>
@@ -570,8 +528,8 @@
   <dimension ref="A1:Y228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I218" sqref="I218"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,28 +549,28 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -671,25 +629,25 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -740,7 +698,7 @@
         <v>2400</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -748,25 +706,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -817,7 +775,7 @@
         <v>2400</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -825,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -902,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
         <v>7.4999999999999997E-2</v>
@@ -979,7 +937,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
         <v>7.4999999999999997E-2</v>
@@ -1056,7 +1014,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>0.375</v>
@@ -1133,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
         <v>1.9</v>
@@ -1210,7 +1168,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2">
         <v>9</v>
@@ -1287,7 +1245,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2">
         <v>7.4999999999999997E-2</v>
@@ -1364,7 +1322,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
         <v>0.375</v>
@@ -1441,7 +1399,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>1.9</v>
@@ -1518,7 +1476,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>9</v>
@@ -1595,7 +1553,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <v>7.4999999999999997E-2</v>
@@ -1672,7 +1630,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
         <v>0.375</v>
@@ -1749,7 +1707,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>1.9</v>
@@ -1826,7 +1784,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2">
         <v>9</v>
@@ -1903,7 +1861,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2">
         <v>9</v>
@@ -1980,7 +1938,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -1989,7 +1947,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F19" s="4">
         <v>0.45</v>
@@ -2054,10 +2012,10 @@
     </row>
     <row r="20" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4">
         <v>9</v>
@@ -2066,7 +2024,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F20" s="4">
         <v>0.45</v>
@@ -2131,10 +2089,10 @@
     </row>
     <row r="21" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4">
         <v>7.4999999999999997E-2</v>
@@ -2143,7 +2101,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F21" s="4">
         <v>0.45</v>
@@ -2208,10 +2166,10 @@
     </row>
     <row r="22" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4">
         <v>0.375</v>
@@ -2220,7 +2178,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F22" s="4">
         <v>0.45</v>
@@ -2285,10 +2243,10 @@
     </row>
     <row r="23" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4">
         <v>1.9</v>
@@ -2297,7 +2255,7 @@
         <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F23" s="4">
         <v>0.45</v>
@@ -2362,10 +2320,10 @@
     </row>
     <row r="24" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C24" s="4">
         <v>9</v>
@@ -2374,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F24" s="4">
         <v>0.45</v>
@@ -2439,10 +2397,10 @@
     </row>
     <row r="25" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4">
         <v>7.4999999999999997E-2</v>
@@ -2451,7 +2409,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F25" s="4">
         <v>0.45</v>
@@ -2516,10 +2474,10 @@
     </row>
     <row r="26" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4">
         <v>0.375</v>
@@ -2528,7 +2486,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F26" s="4">
         <v>0.45</v>
@@ -2593,10 +2551,10 @@
     </row>
     <row r="27" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4">
         <v>1.9</v>
@@ -2605,7 +2563,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F27" s="4">
         <v>0.45</v>
@@ -2670,10 +2628,10 @@
     </row>
     <row r="28" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4">
         <v>9</v>
@@ -2682,7 +2640,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F28" s="4">
         <v>0.45</v>
@@ -2747,10 +2705,10 @@
     </row>
     <row r="29" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C29" s="4">
         <v>7.4999999999999997E-2</v>
@@ -2759,7 +2717,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F29" s="4">
         <v>0.45</v>
@@ -2824,10 +2782,10 @@
     </row>
     <row r="30" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4">
         <v>0.375</v>
@@ -2836,7 +2794,7 @@
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F30" s="4">
         <v>0.45</v>
@@ -2901,10 +2859,10 @@
     </row>
     <row r="31" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4">
         <v>1.9</v>
@@ -2913,7 +2871,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F31" s="4">
         <v>0.45</v>
@@ -2978,10 +2936,10 @@
     </row>
     <row r="32" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4">
         <v>9</v>
@@ -2990,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F32" s="4">
         <v>0.45</v>
@@ -3055,10 +3013,10 @@
     </row>
     <row r="33" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4">
         <v>7.4999999999999997E-2</v>
@@ -3067,7 +3025,7 @@
         <v>10</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F33" s="4">
         <v>0.45</v>
@@ -3132,10 +3090,10 @@
     </row>
     <row r="34" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -3209,10 +3167,10 @@
     </row>
     <row r="35" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2">
         <v>9</v>
@@ -3286,10 +3244,10 @@
     </row>
     <row r="36" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C36" s="2">
         <v>7.4999999999999997E-2</v>
@@ -3363,10 +3321,10 @@
     </row>
     <row r="37" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C37" s="2">
         <v>0.375</v>
@@ -3440,10 +3398,10 @@
     </row>
     <row r="38" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2">
         <v>1.9</v>
@@ -3517,10 +3475,10 @@
     </row>
     <row r="39" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C39" s="2">
         <v>9</v>
@@ -3594,10 +3552,10 @@
     </row>
     <row r="40" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C40" s="2">
         <v>7.4999999999999997E-2</v>
@@ -3671,10 +3629,10 @@
     </row>
     <row r="41" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2">
         <v>0.375</v>
@@ -3748,10 +3706,10 @@
     </row>
     <row r="42" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C42" s="2">
         <v>1.9</v>
@@ -3825,10 +3783,10 @@
     </row>
     <row r="43" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C43" s="2">
         <v>9</v>
@@ -3902,10 +3860,10 @@
     </row>
     <row r="44" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C44" s="2">
         <v>7.4999999999999997E-2</v>
@@ -3979,10 +3937,10 @@
     </row>
     <row r="45" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C45" s="2">
         <v>0.375</v>
@@ -4056,10 +4014,10 @@
     </row>
     <row r="46" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C46" s="2">
         <v>1.9</v>
@@ -4133,10 +4091,10 @@
     </row>
     <row r="47" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C47" s="2">
         <v>9</v>
@@ -4210,10 +4168,10 @@
     </row>
     <row r="48" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C48" s="2">
         <v>9</v>
@@ -4287,10 +4245,10 @@
     </row>
     <row r="49" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3">
         <v>0</v>
@@ -4364,10 +4322,10 @@
     </row>
     <row r="50" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C50" s="3">
         <v>9</v>
@@ -4441,10 +4399,10 @@
     </row>
     <row r="51" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C51" s="3">
         <v>7.4999999999999997E-2</v>
@@ -4518,10 +4476,10 @@
     </row>
     <row r="52" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C52" s="3">
         <v>0.375</v>
@@ -4595,10 +4553,10 @@
     </row>
     <row r="53" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C53" s="3">
         <v>1.9</v>
@@ -4672,10 +4630,10 @@
     </row>
     <row r="54" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C54" s="3">
         <v>9</v>
@@ -4749,10 +4707,10 @@
     </row>
     <row r="55" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C55" s="3">
         <v>7.4999999999999997E-2</v>
@@ -4826,10 +4784,10 @@
     </row>
     <row r="56" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C56" s="3">
         <v>0.375</v>
@@ -4903,10 +4861,10 @@
     </row>
     <row r="57" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C57" s="3">
         <v>1.9</v>
@@ -4980,10 +4938,10 @@
     </row>
     <row r="58" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3">
         <v>9</v>
@@ -5057,10 +5015,10 @@
     </row>
     <row r="59" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C59" s="3">
         <v>7.4999999999999997E-2</v>
@@ -5134,10 +5092,10 @@
     </row>
     <row r="60" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C60" s="3">
         <v>0.375</v>
@@ -5211,10 +5169,10 @@
     </row>
     <row r="61" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C61" s="3">
         <v>1.9</v>
@@ -5288,10 +5246,10 @@
     </row>
     <row r="62" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C62" s="3">
         <v>9</v>
@@ -5365,10 +5323,10 @@
     </row>
     <row r="63" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C63" s="3">
         <v>9</v>
@@ -5442,10 +5400,10 @@
     </row>
     <row r="64" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C64" s="5">
         <v>0</v>
@@ -5519,10 +5477,10 @@
     </row>
     <row r="65" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C65" s="5">
         <v>9</v>
@@ -5596,10 +5554,10 @@
     </row>
     <row r="66" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C66" s="5">
         <v>7.4999999999999997E-2</v>
@@ -5673,10 +5631,10 @@
     </row>
     <row r="67" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C67" s="5">
         <v>0.375</v>
@@ -5750,10 +5708,10 @@
     </row>
     <row r="68" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C68" s="5">
         <v>1.9</v>
@@ -5827,10 +5785,10 @@
     </row>
     <row r="69" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C69" s="5">
         <v>9</v>
@@ -5904,10 +5862,10 @@
     </row>
     <row r="70" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C70" s="5">
         <v>7.4999999999999997E-2</v>
@@ -5981,10 +5939,10 @@
     </row>
     <row r="71" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C71" s="5">
         <v>0.375</v>
@@ -6058,10 +6016,10 @@
     </row>
     <row r="72" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C72" s="5">
         <v>1.9</v>
@@ -6135,10 +6093,10 @@
     </row>
     <row r="73" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C73" s="5">
         <v>9</v>
@@ -6212,10 +6170,10 @@
     </row>
     <row r="74" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C74" s="5">
         <v>7.4999999999999997E-2</v>
@@ -6289,10 +6247,10 @@
     </row>
     <row r="75" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C75" s="5">
         <v>0.375</v>
@@ -6366,10 +6324,10 @@
     </row>
     <row r="76" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C76" s="5">
         <v>1.9</v>
@@ -6443,10 +6401,10 @@
     </row>
     <row r="77" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C77" s="5">
         <v>9</v>
@@ -6520,10 +6478,10 @@
     </row>
     <row r="78" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C78" s="5">
         <v>7.4999999999999997E-2</v>
@@ -6597,10 +6555,10 @@
     </row>
     <row r="79" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C79" s="6">
         <v>0</v>
@@ -6674,10 +6632,10 @@
     </row>
     <row r="80" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C80" s="6">
         <v>7.4999999999999997E-2</v>
@@ -6751,10 +6709,10 @@
     </row>
     <row r="81" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C81" s="6">
         <v>7.4999999999999997E-2</v>
@@ -6828,10 +6786,10 @@
     </row>
     <row r="82" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C82" s="6">
         <v>0.375</v>
@@ -6905,10 +6863,10 @@
     </row>
     <row r="83" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C83" s="6">
         <v>1.9</v>
@@ -6982,10 +6940,10 @@
     </row>
     <row r="84" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C84" s="6">
         <v>9</v>
@@ -7059,10 +7017,10 @@
     </row>
     <row r="85" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C85" s="6">
         <v>7.4999999999999997E-2</v>
@@ -7136,10 +7094,10 @@
     </row>
     <row r="86" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C86" s="6">
         <v>0.375</v>
@@ -7213,10 +7171,10 @@
     </row>
     <row r="87" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C87" s="6">
         <v>1.9</v>
@@ -7290,10 +7248,10 @@
     </row>
     <row r="88" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C88" s="6">
         <v>9</v>
@@ -7367,10 +7325,10 @@
     </row>
     <row r="89" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C89" s="6">
         <v>7.4999999999999997E-2</v>
@@ -7444,10 +7402,10 @@
     </row>
     <row r="90" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C90" s="6">
         <v>0.375</v>
@@ -7521,10 +7479,10 @@
     </row>
     <row r="91" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C91" s="6">
         <v>1.9</v>
@@ -7598,10 +7556,10 @@
     </row>
     <row r="92" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C92" s="6">
         <v>9</v>
@@ -7675,10 +7633,10 @@
     </row>
     <row r="93" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C93" s="6">
         <v>7.4999999999999997E-2</v>
@@ -7752,10 +7710,10 @@
     </row>
     <row r="94" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C94" s="5">
         <v>0</v>
@@ -7829,10 +7787,10 @@
     </row>
     <row r="95" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C95" s="5">
         <v>7.4999999999999997E-2</v>
@@ -7906,10 +7864,10 @@
     </row>
     <row r="96" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C96" s="5">
         <v>7.4999999999999997E-2</v>
@@ -7983,10 +7941,10 @@
     </row>
     <row r="97" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C97" s="5">
         <v>0.375</v>
@@ -8060,10 +8018,10 @@
     </row>
     <row r="98" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C98" s="5">
         <v>1.9</v>
@@ -8137,10 +8095,10 @@
     </row>
     <row r="99" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C99" s="5">
         <v>9</v>
@@ -8214,10 +8172,10 @@
     </row>
     <row r="100" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C100" s="5">
         <v>7.4999999999999997E-2</v>
@@ -8291,10 +8249,10 @@
     </row>
     <row r="101" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C101" s="5">
         <v>0.375</v>
@@ -8368,10 +8326,10 @@
     </row>
     <row r="102" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C102" s="5">
         <v>1.9</v>
@@ -8445,10 +8403,10 @@
     </row>
     <row r="103" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C103" s="5">
         <v>9</v>
@@ -8522,10 +8480,10 @@
     </row>
     <row r="104" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C104" s="5">
         <v>7.4999999999999997E-2</v>
@@ -8599,10 +8557,10 @@
     </row>
     <row r="105" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C105" s="5">
         <v>0.375</v>
@@ -8676,10 +8634,10 @@
     </row>
     <row r="106" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C106" s="5">
         <v>1.9</v>
@@ -8753,10 +8711,10 @@
     </row>
     <row r="107" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C107" s="5">
         <v>9</v>
@@ -8830,10 +8788,10 @@
     </row>
     <row r="108" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C108" s="5">
         <v>7.4999999999999997E-2</v>
@@ -8907,10 +8865,10 @@
     </row>
     <row r="109" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C109" s="6">
         <v>0</v>
@@ -8919,7 +8877,7 @@
         <v>5</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F109" s="6">
         <v>0.45</v>
@@ -8984,10 +8942,10 @@
     </row>
     <row r="110" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C110" s="6">
         <v>9</v>
@@ -8996,7 +8954,7 @@
         <v>5</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F110" s="6">
         <v>0.45</v>
@@ -9061,10 +9019,10 @@
     </row>
     <row r="111" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C111" s="6">
         <v>7.4999999999999997E-2</v>
@@ -9073,7 +9031,7 @@
         <v>5</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F111" s="6">
         <v>0.45</v>
@@ -9138,10 +9096,10 @@
     </row>
     <row r="112" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C112" s="6">
         <v>0.375</v>
@@ -9150,7 +9108,7 @@
         <v>5</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F112" s="6">
         <v>0.45</v>
@@ -9215,10 +9173,10 @@
     </row>
     <row r="113" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C113" s="6">
         <v>1.9</v>
@@ -9227,7 +9185,7 @@
         <v>5</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F113" s="6">
         <v>0.45</v>
@@ -9292,10 +9250,10 @@
     </row>
     <row r="114" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C114" s="6">
         <v>9</v>
@@ -9304,7 +9262,7 @@
         <v>5</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F114" s="6">
         <v>0.45</v>
@@ -9369,10 +9327,10 @@
     </row>
     <row r="115" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C115" s="6">
         <v>7.4999999999999997E-2</v>
@@ -9381,7 +9339,7 @@
         <v>5</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F115" s="6">
         <v>0.45</v>
@@ -9446,10 +9404,10 @@
     </row>
     <row r="116" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C116" s="6">
         <v>0.375</v>
@@ -9458,7 +9416,7 @@
         <v>5</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F116" s="6">
         <v>0.45</v>
@@ -9523,10 +9481,10 @@
     </row>
     <row r="117" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C117" s="6">
         <v>1.9</v>
@@ -9535,7 +9493,7 @@
         <v>5</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F117" s="6">
         <v>0.45</v>
@@ -9600,10 +9558,10 @@
     </row>
     <row r="118" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C118" s="6">
         <v>9</v>
@@ -9612,7 +9570,7 @@
         <v>5</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F118" s="6">
         <v>0.45</v>
@@ -9677,10 +9635,10 @@
     </row>
     <row r="119" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C119" s="6">
         <v>7.4999999999999997E-2</v>
@@ -9689,7 +9647,7 @@
         <v>5</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F119" s="6">
         <v>0.45</v>
@@ -9754,10 +9712,10 @@
     </row>
     <row r="120" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C120" s="6">
         <v>0.375</v>
@@ -9766,7 +9724,7 @@
         <v>5</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F120" s="6">
         <v>0.45</v>
@@ -9831,10 +9789,10 @@
     </row>
     <row r="121" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C121" s="6">
         <v>1.9</v>
@@ -9843,7 +9801,7 @@
         <v>5</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F121" s="6">
         <v>0.45</v>
@@ -9908,10 +9866,10 @@
     </row>
     <row r="122" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C122" s="6">
         <v>9</v>
@@ -9920,7 +9878,7 @@
         <v>5</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F122" s="6">
         <v>0.45</v>
@@ -9985,10 +9943,10 @@
     </row>
     <row r="123" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C123" s="6">
         <v>7.4999999999999997E-2</v>
@@ -9997,7 +9955,7 @@
         <v>5</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F123" s="6">
         <v>0.45</v>
@@ -10062,19 +10020,19 @@
     </row>
     <row r="124" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C124" s="5">
         <v>0</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F124" s="5">
         <v>0.45</v>
@@ -10139,19 +10097,19 @@
     </row>
     <row r="125" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C125" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F125" s="5">
         <v>0.45</v>
@@ -10216,19 +10174,19 @@
     </row>
     <row r="126" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C126" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F126" s="5">
         <v>0.45</v>
@@ -10293,19 +10251,19 @@
     </row>
     <row r="127" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C127" s="5">
         <v>0.375</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F127" s="5">
         <v>0.45</v>
@@ -10370,19 +10328,19 @@
     </row>
     <row r="128" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C128" s="5">
         <v>1.9</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F128" s="5">
         <v>0.45</v>
@@ -10447,19 +10405,19 @@
     </row>
     <row r="129" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C129" s="5">
         <v>9</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F129" s="5">
         <v>0.45</v>
@@ -10524,19 +10482,19 @@
     </row>
     <row r="130" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C130" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F130" s="5">
         <v>0.45</v>
@@ -10601,19 +10559,19 @@
     </row>
     <row r="131" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C131" s="5">
         <v>0.375</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F131" s="5">
         <v>0.45</v>
@@ -10678,19 +10636,19 @@
     </row>
     <row r="132" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C132" s="5">
         <v>1.9</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F132" s="5">
         <v>0.45</v>
@@ -10755,19 +10713,19 @@
     </row>
     <row r="133" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C133" s="5">
         <v>9</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F133" s="5">
         <v>0.45</v>
@@ -10832,19 +10790,19 @@
     </row>
     <row r="134" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C134" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F134" s="5">
         <v>0.45</v>
@@ -10909,19 +10867,19 @@
     </row>
     <row r="135" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C135" s="5">
         <v>0.375</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F135" s="5">
         <v>0.45</v>
@@ -10986,19 +10944,19 @@
     </row>
     <row r="136" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C136" s="5">
         <v>1.9</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F136" s="5">
         <v>0.45</v>
@@ -11063,19 +11021,19 @@
     </row>
     <row r="137" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C137" s="5">
         <v>9</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F137" s="5">
         <v>0.45</v>
@@ -11140,19 +11098,19 @@
     </row>
     <row r="138" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C138" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F138" s="5">
         <v>0.45</v>
@@ -11217,10 +11175,10 @@
     </row>
     <row r="139" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C139" s="6">
         <v>0</v>
@@ -11229,7 +11187,7 @@
         <v>8</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F139" s="6">
         <v>0.45</v>
@@ -11294,10 +11252,10 @@
     </row>
     <row r="140" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C140" s="6">
         <v>7.4999999999999997E-2</v>
@@ -11306,7 +11264,7 @@
         <v>8</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F140" s="6">
         <v>0.45</v>
@@ -11371,10 +11329,10 @@
     </row>
     <row r="141" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C141" s="6">
         <v>7.4999999999999997E-2</v>
@@ -11383,7 +11341,7 @@
         <v>8</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F141" s="6">
         <v>0.45</v>
@@ -11448,10 +11406,10 @@
     </row>
     <row r="142" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C142" s="6">
         <v>0.375</v>
@@ -11460,7 +11418,7 @@
         <v>8</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F142" s="6">
         <v>0.45</v>
@@ -11525,10 +11483,10 @@
     </row>
     <row r="143" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C143" s="6">
         <v>1.9</v>
@@ -11537,7 +11495,7 @@
         <v>8</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F143" s="6">
         <v>0.45</v>
@@ -11602,10 +11560,10 @@
     </row>
     <row r="144" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C144" s="6">
         <v>9</v>
@@ -11614,7 +11572,7 @@
         <v>8</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F144" s="6">
         <v>0.45</v>
@@ -11679,10 +11637,10 @@
     </row>
     <row r="145" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C145" s="6">
         <v>7.4999999999999997E-2</v>
@@ -11691,7 +11649,7 @@
         <v>8</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F145" s="6">
         <v>0.45</v>
@@ -11756,10 +11714,10 @@
     </row>
     <row r="146" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C146" s="6">
         <v>0.375</v>
@@ -11768,7 +11726,7 @@
         <v>8</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F146" s="6">
         <v>0.45</v>
@@ -11833,10 +11791,10 @@
     </row>
     <row r="147" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C147" s="6">
         <v>1.9</v>
@@ -11845,7 +11803,7 @@
         <v>8</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F147" s="6">
         <v>0.45</v>
@@ -11910,10 +11868,10 @@
     </row>
     <row r="148" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C148" s="6">
         <v>9</v>
@@ -11922,7 +11880,7 @@
         <v>8</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F148" s="6">
         <v>0.45</v>
@@ -11987,10 +11945,10 @@
     </row>
     <row r="149" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C149" s="6">
         <v>7.4999999999999997E-2</v>
@@ -11999,7 +11957,7 @@
         <v>8</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F149" s="6">
         <v>0.45</v>
@@ -12064,10 +12022,10 @@
     </row>
     <row r="150" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C150" s="6">
         <v>0.375</v>
@@ -12076,7 +12034,7 @@
         <v>8</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F150" s="6">
         <v>0.45</v>
@@ -12141,10 +12099,10 @@
     </row>
     <row r="151" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C151" s="6">
         <v>1.9</v>
@@ -12153,7 +12111,7 @@
         <v>8</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F151" s="6">
         <v>0.45</v>
@@ -12218,10 +12176,10 @@
     </row>
     <row r="152" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C152" s="6">
         <v>9</v>
@@ -12230,7 +12188,7 @@
         <v>8</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F152" s="6">
         <v>0.45</v>
@@ -12295,10 +12253,10 @@
     </row>
     <row r="153" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C153" s="6">
         <v>7.4999999999999997E-2</v>
@@ -12307,7 +12265,7 @@
         <v>8</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F153" s="6">
         <v>0.45</v>
@@ -12372,10 +12330,10 @@
     </row>
     <row r="154" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C154" s="5">
         <v>0</v>
@@ -12384,7 +12342,7 @@
         <v>8</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F154" s="5">
         <v>0.45</v>
@@ -12449,10 +12407,10 @@
     </row>
     <row r="155" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C155" s="5">
         <v>7.4999999999999997E-2</v>
@@ -12461,7 +12419,7 @@
         <v>8</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F155" s="5">
         <v>0.45</v>
@@ -12526,10 +12484,10 @@
     </row>
     <row r="156" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C156" s="5">
         <v>7.4999999999999997E-2</v>
@@ -12538,7 +12496,7 @@
         <v>8</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F156" s="5">
         <v>0.45</v>
@@ -12603,10 +12561,10 @@
     </row>
     <row r="157" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C157" s="5">
         <v>0.375</v>
@@ -12615,7 +12573,7 @@
         <v>8</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F157" s="5">
         <v>0.45</v>
@@ -12680,10 +12638,10 @@
     </row>
     <row r="158" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C158" s="5">
         <v>1.9</v>
@@ -12692,7 +12650,7 @@
         <v>8</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F158" s="5">
         <v>0.45</v>
@@ -12757,10 +12715,10 @@
     </row>
     <row r="159" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C159" s="5">
         <v>9</v>
@@ -12769,7 +12727,7 @@
         <v>8</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F159" s="5">
         <v>0.45</v>
@@ -12834,10 +12792,10 @@
     </row>
     <row r="160" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C160" s="5">
         <v>7.4999999999999997E-2</v>
@@ -12846,7 +12804,7 @@
         <v>8</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F160" s="5">
         <v>0.45</v>
@@ -12911,10 +12869,10 @@
     </row>
     <row r="161" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C161" s="5">
         <v>0.375</v>
@@ -12923,7 +12881,7 @@
         <v>8</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F161" s="5">
         <v>0.45</v>
@@ -12988,10 +12946,10 @@
     </row>
     <row r="162" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C162" s="5">
         <v>1.9</v>
@@ -13000,7 +12958,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F162" s="5">
         <v>0.45</v>
@@ -13065,10 +13023,10 @@
     </row>
     <row r="163" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C163" s="5">
         <v>9</v>
@@ -13077,7 +13035,7 @@
         <v>8</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F163" s="5">
         <v>0.45</v>
@@ -13142,10 +13100,10 @@
     </row>
     <row r="164" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C164" s="5">
         <v>7.4999999999999997E-2</v>
@@ -13154,7 +13112,7 @@
         <v>8</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F164" s="5">
         <v>0.45</v>
@@ -13219,10 +13177,10 @@
     </row>
     <row r="165" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C165" s="5">
         <v>0.375</v>
@@ -13231,7 +13189,7 @@
         <v>8</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F165" s="5">
         <v>0.45</v>
@@ -13296,10 +13254,10 @@
     </row>
     <row r="166" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C166" s="5">
         <v>1.9</v>
@@ -13308,7 +13266,7 @@
         <v>8</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F166" s="5">
         <v>0.45</v>
@@ -13373,10 +13331,10 @@
     </row>
     <row r="167" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C167" s="5">
         <v>9</v>
@@ -13385,7 +13343,7 @@
         <v>8</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F167" s="5">
         <v>0.45</v>
@@ -13450,10 +13408,10 @@
     </row>
     <row r="168" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C168" s="5">
         <v>9</v>
@@ -13462,7 +13420,7 @@
         <v>8</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F168" s="5">
         <v>0.45</v>
@@ -13527,10 +13485,10 @@
     </row>
     <row r="169" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C169" s="6">
         <v>0</v>
@@ -13539,7 +13497,7 @@
         <v>10</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F169" s="6">
         <v>0.45</v>
@@ -13604,10 +13562,10 @@
     </row>
     <row r="170" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C170" s="6">
         <v>9</v>
@@ -13616,7 +13574,7 @@
         <v>10</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F170" s="6">
         <v>0.45</v>
@@ -13681,10 +13639,10 @@
     </row>
     <row r="171" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C171" s="6">
         <v>7.4999999999999997E-2</v>
@@ -13693,7 +13651,7 @@
         <v>10</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F171" s="6">
         <v>0.45</v>
@@ -13758,10 +13716,10 @@
     </row>
     <row r="172" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C172" s="6">
         <v>0.375</v>
@@ -13770,7 +13728,7 @@
         <v>10</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F172" s="6">
         <v>0.45</v>
@@ -13835,10 +13793,10 @@
     </row>
     <row r="173" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C173" s="6">
         <v>1.9</v>
@@ -13847,7 +13805,7 @@
         <v>10</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F173" s="6">
         <v>0.45</v>
@@ -13912,10 +13870,10 @@
     </row>
     <row r="174" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C174" s="6">
         <v>9</v>
@@ -13924,7 +13882,7 @@
         <v>10</v>
       </c>
       <c r="E174" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F174" s="6">
         <v>0.45</v>
@@ -13989,10 +13947,10 @@
     </row>
     <row r="175" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C175" s="6">
         <v>7.4999999999999997E-2</v>
@@ -14001,7 +13959,7 @@
         <v>10</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F175" s="6">
         <v>0.45</v>
@@ -14066,10 +14024,10 @@
     </row>
     <row r="176" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C176" s="6">
         <v>0.375</v>
@@ -14078,7 +14036,7 @@
         <v>10</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F176" s="6">
         <v>0.45</v>
@@ -14143,10 +14101,10 @@
     </row>
     <row r="177" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C177" s="6">
         <v>1.9</v>
@@ -14155,7 +14113,7 @@
         <v>10</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F177" s="6">
         <v>0.45</v>
@@ -14220,10 +14178,10 @@
     </row>
     <row r="178" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C178" s="6">
         <v>9</v>
@@ -14232,7 +14190,7 @@
         <v>10</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F178" s="6">
         <v>0.45</v>
@@ -14297,10 +14255,10 @@
     </row>
     <row r="179" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C179" s="6">
         <v>7.4999999999999997E-2</v>
@@ -14309,7 +14267,7 @@
         <v>10</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F179" s="6">
         <v>0.45</v>
@@ -14374,10 +14332,10 @@
     </row>
     <row r="180" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C180" s="6">
         <v>0.375</v>
@@ -14386,7 +14344,7 @@
         <v>10</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F180" s="6">
         <v>0.45</v>
@@ -14451,10 +14409,10 @@
     </row>
     <row r="181" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C181" s="6">
         <v>1.9</v>
@@ -14463,7 +14421,7 @@
         <v>10</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F181" s="6">
         <v>0.45</v>
@@ -14528,10 +14486,10 @@
     </row>
     <row r="182" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C182" s="6">
         <v>9</v>
@@ -14540,7 +14498,7 @@
         <v>10</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F182" s="6">
         <v>0.45</v>
@@ -14605,10 +14563,10 @@
     </row>
     <row r="183" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C183" s="6">
         <v>9</v>
@@ -14617,7 +14575,7 @@
         <v>10</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F183" s="6">
         <v>0.45</v>
@@ -14682,10 +14640,10 @@
     </row>
     <row r="184" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C184" s="5">
         <v>0</v>
@@ -14694,7 +14652,7 @@
         <v>11</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F184" s="5">
         <v>0.45</v>
@@ -14759,10 +14717,10 @@
     </row>
     <row r="185" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C185" s="5">
         <v>7.4999999999999997E-2</v>
@@ -14771,7 +14729,7 @@
         <v>11</v>
       </c>
       <c r="E185" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F185" s="5">
         <v>0.45</v>
@@ -14836,10 +14794,10 @@
     </row>
     <row r="186" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C186" s="5">
         <v>7.4999999999999997E-2</v>
@@ -14848,7 +14806,7 @@
         <v>11</v>
       </c>
       <c r="E186" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F186" s="5">
         <v>0.45</v>
@@ -14913,10 +14871,10 @@
     </row>
     <row r="187" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C187" s="5">
         <v>0.375</v>
@@ -14925,7 +14883,7 @@
         <v>11</v>
       </c>
       <c r="E187" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F187" s="5">
         <v>0.45</v>
@@ -14990,10 +14948,10 @@
     </row>
     <row r="188" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C188" s="5">
         <v>1.9</v>
@@ -15002,7 +14960,7 @@
         <v>11</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F188" s="5">
         <v>0.45</v>
@@ -15067,10 +15025,10 @@
     </row>
     <row r="189" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C189" s="5">
         <v>9</v>
@@ -15079,7 +15037,7 @@
         <v>11</v>
       </c>
       <c r="E189" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F189" s="5">
         <v>0.45</v>
@@ -15144,10 +15102,10 @@
     </row>
     <row r="190" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C190" s="5">
         <v>7.4999999999999997E-2</v>
@@ -15156,7 +15114,7 @@
         <v>11</v>
       </c>
       <c r="E190" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F190" s="5">
         <v>0.45</v>
@@ -15221,10 +15179,10 @@
     </row>
     <row r="191" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C191" s="5">
         <v>0.375</v>
@@ -15233,7 +15191,7 @@
         <v>11</v>
       </c>
       <c r="E191" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F191" s="5">
         <v>0.45</v>
@@ -15298,10 +15256,10 @@
     </row>
     <row r="192" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C192" s="5">
         <v>1.9</v>
@@ -15310,7 +15268,7 @@
         <v>11</v>
       </c>
       <c r="E192" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F192" s="5">
         <v>0.45</v>
@@ -15375,10 +15333,10 @@
     </row>
     <row r="193" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C193" s="5">
         <v>9</v>
@@ -15387,7 +15345,7 @@
         <v>11</v>
       </c>
       <c r="E193" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F193" s="5">
         <v>0.45</v>
@@ -15452,10 +15410,10 @@
     </row>
     <row r="194" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C194" s="5">
         <v>7.4999999999999997E-2</v>
@@ -15464,7 +15422,7 @@
         <v>11</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F194" s="5">
         <v>0.45</v>
@@ -15529,10 +15487,10 @@
     </row>
     <row r="195" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C195" s="5">
         <v>0.375</v>
@@ -15541,7 +15499,7 @@
         <v>11</v>
       </c>
       <c r="E195" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F195" s="5">
         <v>0.45</v>
@@ -15606,10 +15564,10 @@
     </row>
     <row r="196" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C196" s="5">
         <v>1.9</v>
@@ -15618,7 +15576,7 @@
         <v>11</v>
       </c>
       <c r="E196" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F196" s="5">
         <v>0.45</v>
@@ -15683,10 +15641,10 @@
     </row>
     <row r="197" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C197" s="5">
         <v>9</v>
@@ -15695,7 +15653,7 @@
         <v>11</v>
       </c>
       <c r="E197" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F197" s="5">
         <v>0.45</v>
@@ -15760,10 +15718,10 @@
     </row>
     <row r="198" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C198" s="5">
         <v>9</v>
@@ -15772,7 +15730,7 @@
         <v>11</v>
       </c>
       <c r="E198" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F198" s="5">
         <v>0.45</v>
@@ -15837,10 +15795,10 @@
     </row>
     <row r="199" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C199" s="6">
         <v>0</v>
@@ -15849,7 +15807,7 @@
         <v>12</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F199" s="6">
         <v>0.45</v>
@@ -15914,10 +15872,10 @@
     </row>
     <row r="200" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C200" s="6">
         <v>9</v>
@@ -15926,7 +15884,7 @@
         <v>12</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F200" s="6">
         <v>0.45</v>
@@ -15991,10 +15949,10 @@
     </row>
     <row r="201" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C201" s="6">
         <v>7.4999999999999997E-2</v>
@@ -16003,7 +15961,7 @@
         <v>12</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F201" s="6">
         <v>0.45</v>
@@ -16068,10 +16026,10 @@
     </row>
     <row r="202" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C202" s="6">
         <v>0.375</v>
@@ -16080,7 +16038,7 @@
         <v>12</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F202" s="6">
         <v>0.45</v>
@@ -16145,10 +16103,10 @@
     </row>
     <row r="203" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C203" s="6">
         <v>1.9</v>
@@ -16157,7 +16115,7 @@
         <v>12</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F203" s="6">
         <v>0.45</v>
@@ -16222,10 +16180,10 @@
     </row>
     <row r="204" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C204" s="6">
         <v>9</v>
@@ -16234,7 +16192,7 @@
         <v>12</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F204" s="6">
         <v>0.45</v>
@@ -16299,10 +16257,10 @@
     </row>
     <row r="205" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C205" s="6">
         <v>7.4999999999999997E-2</v>
@@ -16311,7 +16269,7 @@
         <v>12</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F205" s="6">
         <v>0.45</v>
@@ -16376,10 +16334,10 @@
     </row>
     <row r="206" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C206" s="6">
         <v>0.375</v>
@@ -16388,7 +16346,7 @@
         <v>12</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F206" s="6">
         <v>0.45</v>
@@ -16453,10 +16411,10 @@
     </row>
     <row r="207" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C207" s="6">
         <v>1.9</v>
@@ -16465,7 +16423,7 @@
         <v>12</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F207" s="6">
         <v>0.45</v>
@@ -16530,10 +16488,10 @@
     </row>
     <row r="208" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C208" s="6">
         <v>9</v>
@@ -16542,7 +16500,7 @@
         <v>12</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F208" s="6">
         <v>0.45</v>
@@ -16607,10 +16565,10 @@
     </row>
     <row r="209" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C209" s="6">
         <v>7.4999999999999997E-2</v>
@@ -16619,7 +16577,7 @@
         <v>12</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F209" s="6">
         <v>0.45</v>
@@ -16684,10 +16642,10 @@
     </row>
     <row r="210" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C210" s="6">
         <v>0.375</v>
@@ -16696,7 +16654,7 @@
         <v>12</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F210" s="6">
         <v>0.45</v>
@@ -16761,10 +16719,10 @@
     </row>
     <row r="211" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C211" s="6">
         <v>1.9</v>
@@ -16773,7 +16731,7 @@
         <v>12</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F211" s="6">
         <v>0.45</v>
@@ -16838,10 +16796,10 @@
     </row>
     <row r="212" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C212" s="6">
         <v>9</v>
@@ -16850,7 +16808,7 @@
         <v>12</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F212" s="6">
         <v>0.45</v>
@@ -16915,10 +16873,10 @@
     </row>
     <row r="213" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C213" s="6">
         <v>9</v>
@@ -16927,7 +16885,7 @@
         <v>12</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F213" s="6">
         <v>0.45</v>
@@ -16992,10 +16950,10 @@
     </row>
     <row r="214" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C214" s="5">
         <v>0</v>
@@ -17069,10 +17027,10 @@
     </row>
     <row r="215" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C215" s="5">
         <v>9</v>
@@ -17146,10 +17104,10 @@
     </row>
     <row r="216" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C216" s="5">
         <v>7.4999999999999997E-2</v>
@@ -17223,10 +17181,10 @@
     </row>
     <row r="217" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C217" s="5">
         <v>0.375</v>
@@ -17300,10 +17258,10 @@
     </row>
     <row r="218" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C218" s="5">
         <v>1.9</v>
@@ -17377,10 +17335,10 @@
     </row>
     <row r="219" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C219" s="5">
         <v>9</v>
@@ -17454,10 +17412,10 @@
     </row>
     <row r="220" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C220" s="5">
         <v>7.4999999999999997E-2</v>
@@ -17531,10 +17489,10 @@
     </row>
     <row r="221" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C221" s="5">
         <v>0.375</v>
@@ -17608,10 +17566,10 @@
     </row>
     <row r="222" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C222" s="5">
         <v>1.9</v>
@@ -17685,10 +17643,10 @@
     </row>
     <row r="223" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C223" s="5">
         <v>9</v>
@@ -17762,10 +17720,10 @@
     </row>
     <row r="224" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C224" s="5">
         <v>7.4999999999999997E-2</v>
@@ -17839,10 +17797,10 @@
     </row>
     <row r="225" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C225" s="5">
         <v>0.375</v>
@@ -17916,10 +17874,10 @@
     </row>
     <row r="226" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C226" s="5">
         <v>1.9</v>
@@ -17993,10 +17951,10 @@
     </row>
     <row r="227" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C227" s="5">
         <v>9</v>
@@ -18070,10 +18028,10 @@
     </row>
     <row r="228" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C228" s="5">
         <v>9</v>

</xml_diff>